<commit_message>
Begin developing waffle plot to replace wind roses
</commit_message>
<xml_diff>
--- a/io_in/colors.xlsx
+++ b/io_in/colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776DEB7D-D598-F242-A89B-AEA4950AD519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B86DA1-DEE0-7946-B934-50A825DB9BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{BDCAF731-B127-1140-A939-934C8A5530D0}"/>
+    <workbookView xWindow="7800" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{BDCAF731-B127-1140-A939-934C8A5530D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>